<commit_message>
update hour log and readme
</commit_message>
<xml_diff>
--- a/DTT-Assessment-Hour-Log.xlsx
+++ b/DTT-Assessment-Hour-Log.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <r>
       <rPr>
@@ -74,11 +74,21 @@
     <r>
       <rPr>
         <sz val="8"/>
+        <color rgb="FFC9211E"/>
         <rFont val="Open Sans"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Since I already applied once for an internship with DTT, and that time I had to make a very similar assignment (Including maze generation using Aldous-Broder, Binary Tree, and Prim’s Algorrithm, Random Depth First Search, my project from that time can be found at </t>
+      <t xml:space="preserve">Since I already applied once for an internship with DTT, and that time I had to make a very similar assignment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Including maze generation using Aldous-Broder, Binary Tree, and Prim’s Algorrithm, Random Depth First Search, my project from that time can be found at </t>
     </r>
     <r>
       <rPr>
@@ -97,7 +107,26 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> ), this time I want to focus on the visualization and gameplay more than the maze generation itself. Thus, I looked at the results of a view perfect maze algorithms and picked the most visually interesting that I haven’t programmed before, Recursive Division. Steps on how that algorithm works are listed at </t>
+      <t xml:space="preserve"> ), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFC9211E"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">this time I want to focus on supporting both 2d and 3d generation, and to have a player solve the 3d generated maze.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> I looked at the results of a few perfect maze algorithms and picked the most visually interesting that I haven’t programmed before, Recursive Division. Steps on how that algorithm works are listed at </t>
     </r>
     <r>
       <rPr>
@@ -240,6 +269,21 @@
     <t xml:space="preserve">I playtested and fixed any bugs I could find. I fixed things such as input validation, and made a lot of final tweaks, like being able to restart the game, toggling UI elements in the 3d mode etc. These changes are too small to individually sum in a list, but these small things really make for a better user experience.</t>
   </si>
   <si>
+    <t xml:space="preserve">Refactor, build and document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22/05/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I refactored a bunch of code that wasn’t neat, removed the need for serializing a lot of dependencies by resolving these through code, then added comments wherever required. I made a build, did a final playtest, and updated the hour log and trello board.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What I would improve given more time…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There’s many things to improve, but I delivered a functional prototype. I would improve the visuals by altering the used materials, add different maze generation algorithms (again, I did make it possible to easily add new generation aglorithms, but haven’t decided to add additional generation algorithms as I have already shown how I would add those in the old assessment ( github.com/kemmel-dev/MazeGen )), and add some more interesting scenery and gameplay elements. It would also be fun to have a second player do a maze-race! Mostly the aesthethics should get an overhaul, including sound design.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Total amount of hours</t>
   </si>
 </sst>
@@ -253,7 +297,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -323,6 +367,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC9211E"/>
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
@@ -466,7 +517,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,15 +570,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -624,7 +679,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -644,9 +699,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2217240</xdr:colOff>
+      <xdr:colOff>2216520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>819360</xdr:rowOff>
+      <xdr:rowOff>818640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -660,7 +715,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="148320" y="131760"/>
-          <a:ext cx="2068920" cy="687600"/>
+          <a:ext cx="2068200" cy="686880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -682,8 +737,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,7 +786,7 @@
       </c>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>6</v>
       </c>
@@ -773,7 +828,7 @@
       <c r="C6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="12"/>
@@ -789,7 +844,7 @@
       <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="12"/>
@@ -805,7 +860,7 @@
       <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="12"/>
@@ -821,7 +876,7 @@
       <c r="C9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="12"/>
@@ -837,7 +892,7 @@
       <c r="C10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="12"/>
@@ -853,7 +908,7 @@
       <c r="C11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="12"/>
@@ -869,7 +924,7 @@
       <c r="C12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="12"/>
@@ -885,7 +940,7 @@
       <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="15" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="12" t="s">
@@ -903,7 +958,7 @@
       <c r="C14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="15" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -921,7 +976,7 @@
       <c r="C15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="15" t="s">
         <v>34</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -939,7 +994,7 @@
       <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="15" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="12"/>
@@ -955,7 +1010,7 @@
       <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="15" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -973,7 +1028,7 @@
       <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="15" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="12" t="s">
@@ -991,7 +1046,7 @@
       <c r="C19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="15" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="12" t="s">
@@ -999,11 +1054,19 @@
       </c>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="13"/>
+    <row r="20" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="E20" s="12"/>
       <c r="F20" s="7"/>
     </row>
@@ -1011,7 +1074,7 @@
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="15"/>
       <c r="E21" s="12"/>
       <c r="F21" s="7"/>
     </row>
@@ -1019,15 +1082,19 @@
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="12"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8"/>
+    <row r="23" customFormat="false" ht="73.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="15" t="s">
+        <v>49</v>
+      </c>
       <c r="E23" s="12"/>
       <c r="F23" s="7"/>
     </row>
@@ -1035,7 +1102,7 @@
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="15"/>
       <c r="E24" s="12"/>
       <c r="F24" s="7"/>
     </row>
@@ -1043,7 +1110,7 @@
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="12"/>
       <c r="F25" s="7"/>
     </row>
@@ -1051,7 +1118,7 @@
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="15"/>
       <c r="E26" s="12"/>
       <c r="F26" s="7"/>
     </row>
@@ -1059,7 +1126,7 @@
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="13"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="12"/>
       <c r="F27" s="7"/>
     </row>
@@ -1067,54 +1134,54 @@
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="15"/>
       <c r="E28" s="12"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="18" t="n">
+      <c r="A30" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="19" t="n">
         <f aca="false">SUM(B4:B28)</f>
-        <v>19</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="19"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="22"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>